<commit_message>
Modified after 5 min
</commit_message>
<xml_diff>
--- a/live_crypto_data.xlsx
+++ b/live_crypto_data.xlsx
@@ -478,16 +478,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>93868.67548097557</v>
+        <v>93593.70593424888</v>
       </c>
       <c r="D2" t="n">
-        <v>1858612352925.831</v>
+        <v>1853167919054.723</v>
       </c>
       <c r="E2" t="n">
-        <v>59599375918.81479</v>
+        <v>59748244183.16138</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.83058014</v>
+        <v>-2.16511306</v>
       </c>
     </row>
     <row r="3">
@@ -502,16 +502,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3374.139607770159</v>
+        <v>3352.555608610053</v>
       </c>
       <c r="D3" t="n">
-        <v>406439580895.5662</v>
+        <v>403839631695.9297</v>
       </c>
       <c r="E3" t="n">
-        <v>32434492743.43126</v>
+        <v>32513038434.96328</v>
       </c>
       <c r="F3" t="n">
-        <v>1.39229033</v>
+        <v>0.6943679699999999</v>
       </c>
     </row>
     <row r="4">
@@ -526,16 +526,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9986787548714428</v>
+        <v>0.9986123728111663</v>
       </c>
       <c r="D4" t="n">
-        <v>139663496085.7792</v>
+        <v>139654212669.495</v>
       </c>
       <c r="E4" t="n">
-        <v>134528538899.5783</v>
+        <v>134856672030.5432</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.05398583</v>
+        <v>-0.08507927</v>
       </c>
     </row>
     <row r="5">
@@ -550,16 +550,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2.195052655547284</v>
+        <v>2.190784119817687</v>
       </c>
       <c r="D5" t="n">
-        <v>125671989677.3243</v>
+        <v>125427605845.8971</v>
       </c>
       <c r="E5" t="n">
-        <v>10919366585.31427</v>
+        <v>10926323035.3287</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.94666203</v>
+        <v>-2.13208952</v>
       </c>
     </row>
     <row r="6">
@@ -574,16 +574,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>683.3349340120989</v>
+        <v>681.414910328032</v>
       </c>
       <c r="D6" t="n">
-        <v>98405417727.39308</v>
+        <v>98128919741.89166</v>
       </c>
       <c r="E6" t="n">
-        <v>1682453033.670772</v>
+        <v>1680950145.051784</v>
       </c>
       <c r="F6" t="n">
-        <v>3.93443311</v>
+        <v>3.53900119</v>
       </c>
     </row>
     <row r="7">
@@ -598,16 +598,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>185.1549030497088</v>
+        <v>185.0009753963551</v>
       </c>
       <c r="D7" t="n">
-        <v>88774402584.0825</v>
+        <v>88700600404.16412</v>
       </c>
       <c r="E7" t="n">
-        <v>4507261362.902628</v>
+        <v>4520706652.315876</v>
       </c>
       <c r="F7" t="n">
-        <v>1.27077224</v>
+        <v>1.24663073</v>
       </c>
     </row>
     <row r="8">
@@ -622,16 +622,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.3140363181460863</v>
+        <v>0.3133869202417922</v>
       </c>
       <c r="D8" t="n">
-        <v>46264438484.09074</v>
+        <v>46168767927.3466</v>
       </c>
       <c r="E8" t="n">
-        <v>4118383308.390707</v>
+        <v>4122155365.7529</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.8805674</v>
+        <v>-1.0920213</v>
       </c>
     </row>
     <row r="9">
@@ -646,16 +646,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.9999207210033452</v>
+        <v>0.9999344736902294</v>
       </c>
       <c r="D9" t="n">
-        <v>43178629891.02515</v>
+        <v>43179223760.28349</v>
       </c>
       <c r="E9" t="n">
-        <v>9154695826.343916</v>
+        <v>9172186703.4751</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00157308</v>
+        <v>-0.01844355</v>
       </c>
     </row>
     <row r="10">
@@ -670,16 +670,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.8987550089008702</v>
+        <v>0.8959722778375632</v>
       </c>
       <c r="D10" t="n">
-        <v>31569820882.4607</v>
+        <v>31472074199.14585</v>
       </c>
       <c r="E10" t="n">
-        <v>1218927857.441288</v>
+        <v>1222973140.17203</v>
       </c>
       <c r="F10" t="n">
-        <v>0.31538006</v>
+        <v>0.04080606</v>
       </c>
     </row>
     <row r="11">
@@ -694,16 +694,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.2498969924848784</v>
+        <v>0.2498807197361438</v>
       </c>
       <c r="D11" t="n">
-        <v>21544600350.332</v>
+        <v>21543197412.80721</v>
       </c>
       <c r="E11" t="n">
-        <v>1234243900.581338</v>
+        <v>1235717224.513316</v>
       </c>
       <c r="F11" t="n">
-        <v>1.14350128</v>
+        <v>1.14241428</v>
       </c>
     </row>
     <row r="12">
@@ -718,16 +718,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>37.29839822758839</v>
+        <v>37.15734698540833</v>
       </c>
       <c r="D12" t="n">
-        <v>15286213158.83239</v>
+        <v>15228405331.77435</v>
       </c>
       <c r="E12" t="n">
-        <v>636471055.5142049</v>
+        <v>637931089.3408355</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.1312692</v>
+        <v>-0.53231795</v>
       </c>
     </row>
     <row r="13">
@@ -742,16 +742,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>22.97021837932882</v>
+        <v>22.89203701503313</v>
       </c>
       <c r="D13" t="n">
-        <v>14657295669.14378</v>
+        <v>14607408142.89674</v>
       </c>
       <c r="E13" t="n">
-        <v>1083417245.895584</v>
+        <v>1084790623.173182</v>
       </c>
       <c r="F13" t="n">
-        <v>3.36976791</v>
+        <v>3.00272092</v>
       </c>
     </row>
     <row r="14">
@@ -766,16 +766,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5.485241665005813</v>
+        <v>5.480738466563957</v>
       </c>
       <c r="D14" t="n">
-        <v>13997781653.42079</v>
+        <v>13986289946.69558</v>
       </c>
       <c r="E14" t="n">
-        <v>230118586.1281941</v>
+        <v>230554818.6848345</v>
       </c>
       <c r="F14" t="n">
-        <v>1.01914733</v>
+        <v>0.92166012</v>
       </c>
     </row>
     <row r="15">
@@ -790,16 +790,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2.185385543275544e-05</v>
+        <v>2.183443620001012e-05</v>
       </c>
       <c r="D15" t="n">
-        <v>12877503890.40417</v>
+        <v>12866061001.25375</v>
       </c>
       <c r="E15" t="n">
-        <v>657977664.2334504</v>
+        <v>658972883.8270316</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.17740374</v>
+        <v>-0.20632331</v>
       </c>
     </row>
     <row r="16">
@@ -814,16 +814,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4.278948472768872</v>
+        <v>4.269991333044081</v>
       </c>
       <c r="D16" t="n">
-        <v>12527306365.19904</v>
+        <v>12501082905.34613</v>
       </c>
       <c r="E16" t="n">
-        <v>1993849869.504949</v>
+        <v>1995715952.473691</v>
       </c>
       <c r="F16" t="n">
-        <v>-1.03393363</v>
+        <v>-1.32131459</v>
       </c>
     </row>
     <row r="17">
@@ -838,16 +838,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>7.088450648329903</v>
+        <v>7.060517600388184</v>
       </c>
       <c r="D17" t="n">
-        <v>10856927761.49319</v>
+        <v>10814144493.51163</v>
       </c>
       <c r="E17" t="n">
-        <v>419791559.509302</v>
+        <v>421613573.151455</v>
       </c>
       <c r="F17" t="n">
-        <v>1.51731935</v>
+        <v>1.13592866</v>
       </c>
     </row>
     <row r="18">
@@ -862,16 +862,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.3576611391911084</v>
+        <v>0.3572769795416412</v>
       </c>
       <c r="D18" t="n">
-        <v>10811345509.72109</v>
+        <v>10799733169.8659</v>
       </c>
       <c r="E18" t="n">
-        <v>439508708.8029994</v>
+        <v>439595598.3194231</v>
       </c>
       <c r="F18" t="n">
-        <v>-1.02806607</v>
+        <v>-1.06022475</v>
       </c>
     </row>
     <row r="19">
@@ -886,16 +886,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.2723127962353633</v>
+        <v>0.2707210739885201</v>
       </c>
       <c r="D19" t="n">
-        <v>10416553346.03961</v>
+        <v>10355666527.91892</v>
       </c>
       <c r="E19" t="n">
-        <v>1002658804.536276</v>
+        <v>995252051.6471295</v>
       </c>
       <c r="F19" t="n">
-        <v>1.98432343</v>
+        <v>1.31163355</v>
       </c>
     </row>
     <row r="20">
@@ -910,16 +910,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>442.2543592420329</v>
+        <v>441.961743447117</v>
       </c>
       <c r="D20" t="n">
-        <v>8759180657.602766</v>
+        <v>8753385181.408186</v>
       </c>
       <c r="E20" t="n">
-        <v>401042988.9054862</v>
+        <v>401518573.6439794</v>
       </c>
       <c r="F20" t="n">
-        <v>-1.65730281</v>
+        <v>-1.69652879</v>
       </c>
     </row>
     <row r="21">
@@ -934,16 +934,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>9.439150241115231</v>
+        <v>9.421996910912126</v>
       </c>
       <c r="D21" t="n">
-        <v>8725977301.438606</v>
+        <v>8710119987.361288</v>
       </c>
       <c r="E21" t="n">
-        <v>1118049.32086794</v>
+        <v>1120666.48264045</v>
       </c>
       <c r="F21" t="n">
-        <v>1.11598306</v>
+        <v>0.94497427</v>
       </c>
     </row>
     <row r="22">
@@ -958,16 +958,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>13.8376413006066</v>
+        <v>13.81215888022934</v>
       </c>
       <c r="D22" t="n">
-        <v>8309269381.084696</v>
+        <v>8293967618.970984</v>
       </c>
       <c r="E22" t="n">
-        <v>595985933.9789559</v>
+        <v>596263820.7778939</v>
       </c>
       <c r="F22" t="n">
-        <v>-1.59357185</v>
+        <v>-1.68286208</v>
       </c>
     </row>
     <row r="23">
@@ -982,64 +982,64 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>102.3126625668172</v>
+        <v>102.1565761590558</v>
       </c>
       <c r="D23" t="n">
-        <v>7708077367.53677</v>
+        <v>7696318059.579557</v>
       </c>
       <c r="E23" t="n">
-        <v>740280881.0636618</v>
+        <v>740881840.7011844</v>
       </c>
       <c r="F23" t="n">
-        <v>0.60134046</v>
+        <v>0.41680271</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Hyperliquid</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>HYPE</t>
+          <t>PEPE</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>28.09458072956739</v>
+        <v>1.803631128995296e-05</v>
       </c>
       <c r="D24" t="n">
-        <v>7611062605.912917</v>
+        <v>7587693992.939088</v>
       </c>
       <c r="E24" t="n">
-        <v>740125978.1598023</v>
+        <v>2133190220.55208</v>
       </c>
       <c r="F24" t="n">
-        <v>-9.737026630000001</v>
+        <v>-0.33329076</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Hyperliquid</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>PEPE</t>
+          <t>HYPE</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1.807105051537823e-05</v>
+        <v>27.85843433477825</v>
       </c>
       <c r="D25" t="n">
-        <v>7602308434.209321</v>
+        <v>7547088524.498374</v>
       </c>
       <c r="E25" t="n">
-        <v>2133924126.16953</v>
+        <v>740055505.3636495</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.35424239</v>
+        <v>-9.852136570000001</v>
       </c>
     </row>
     <row r="26">
@@ -1054,16 +1054,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.181784941981447</v>
+        <v>5.176209265976165</v>
       </c>
       <c r="D26" t="n">
-        <v>6310927774.725522</v>
+        <v>6304137124.600403</v>
       </c>
       <c r="E26" t="n">
-        <v>930748795.680459</v>
+        <v>931955322.5777456</v>
       </c>
       <c r="F26" t="n">
-        <v>2.25251444</v>
+        <v>2.13008712</v>
       </c>
     </row>
     <row r="27">
@@ -1078,16 +1078,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.998553664733392</v>
+        <v>0.998519221181791</v>
       </c>
       <c r="D27" t="n">
-        <v>5914994086.493386</v>
+        <v>5914790057.995737</v>
       </c>
       <c r="E27" t="n">
-        <v>104551363.9007271</v>
+        <v>104646477.902974</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.0831539</v>
+        <v>-0.08632832</v>
       </c>
     </row>
     <row r="28">
@@ -1102,16 +1102,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>4.06262261486151</v>
+        <v>4.082166220556925</v>
       </c>
       <c r="D28" t="n">
-        <v>5687671660.806114</v>
+        <v>5715032708.779695</v>
       </c>
       <c r="E28" t="n">
-        <v>117337925.2370617</v>
+        <v>118860920.2149833</v>
       </c>
       <c r="F28" t="n">
-        <v>-2.14941298</v>
+        <v>-1.75967283</v>
       </c>
     </row>
     <row r="29">
@@ -1126,16 +1126,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.999672641285563</v>
+        <v>0.9996664115784819</v>
       </c>
       <c r="D29" t="n">
-        <v>5363626297.880865</v>
+        <v>5363592873.11825</v>
       </c>
       <c r="E29" t="n">
-        <v>161761350.1180645</v>
+        <v>161988535.0059164</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.00553862</v>
+        <v>-0.01436735</v>
       </c>
     </row>
     <row r="30">
@@ -1150,16 +1150,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>350.3112017355579</v>
+        <v>350.1955302810284</v>
       </c>
       <c r="D30" t="n">
-        <v>5261064023.838758</v>
+        <v>5259326840.086153</v>
       </c>
       <c r="E30" t="n">
-        <v>1215915427.436319</v>
+        <v>1220682102.293655</v>
       </c>
       <c r="F30" t="n">
-        <v>13.55860911</v>
+        <v>13.72400358</v>
       </c>
     </row>
     <row r="31">
@@ -1174,16 +1174,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>9.327855224614408</v>
+        <v>9.300876569441261</v>
       </c>
       <c r="D31" t="n">
-        <v>5189917272.101545</v>
+        <v>5174906641.566488</v>
       </c>
       <c r="E31" t="n">
-        <v>508618108.0001369</v>
+        <v>508002701.5491415</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.37489808</v>
+        <v>-0.76327685</v>
       </c>
     </row>
     <row r="32">
@@ -1198,16 +1198,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>10.22097465055707</v>
+        <v>10.20095846321917</v>
       </c>
       <c r="D32" t="n">
-        <v>4880491104.969839</v>
+        <v>4870933423.085492</v>
       </c>
       <c r="E32" t="n">
-        <v>195264820.7970554</v>
+        <v>195140183.5938376</v>
       </c>
       <c r="F32" t="n">
-        <v>1.98354825</v>
+        <v>1.75047501</v>
       </c>
     </row>
     <row r="33">
@@ -1222,16 +1222,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.1575327195190269</v>
+        <v>0.1574520449695216</v>
       </c>
       <c r="D33" t="n">
-        <v>4185890218.305768</v>
+        <v>4183746569.616963</v>
       </c>
       <c r="E33" t="n">
-        <v>36246037.74842487</v>
+        <v>36328265.03279613</v>
       </c>
       <c r="F33" t="n">
-        <v>-0.24506346</v>
+        <v>-0.24622047</v>
       </c>
     </row>
     <row r="34">
@@ -1246,16 +1246,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.4811655873904274</v>
+        <v>0.4802348569379254</v>
       </c>
       <c r="D34" t="n">
-        <v>4040081897.305357</v>
+        <v>4032267067.336287</v>
       </c>
       <c r="E34" t="n">
-        <v>241788043.0225672</v>
+        <v>241914602.8810993</v>
       </c>
       <c r="F34" t="n">
-        <v>0.21714924</v>
+        <v>0.10246063</v>
       </c>
     </row>
     <row r="35">
@@ -1270,16 +1270,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>26.58422584091222</v>
+        <v>26.52573272841433</v>
       </c>
       <c r="D35" t="n">
-        <v>3989260267.338838</v>
+        <v>3980482721.925358</v>
       </c>
       <c r="E35" t="n">
-        <v>255995353.9374411</v>
+        <v>256630611.4218283</v>
       </c>
       <c r="F35" t="n">
-        <v>1.04143583</v>
+        <v>0.88244808</v>
       </c>
     </row>
     <row r="36">
@@ -1294,16 +1294,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1.178926944456939</v>
+        <v>1.178787309293449</v>
       </c>
       <c r="D36" t="n">
-        <v>3969260407.090267</v>
+        <v>3968790277.59795</v>
       </c>
       <c r="E36" t="n">
-        <v>146034600.6469674</v>
+        <v>146169415.3803568</v>
       </c>
       <c r="F36" t="n">
-        <v>0.15402369</v>
+        <v>0.18555388</v>
       </c>
     </row>
     <row r="37">
@@ -1318,16 +1318,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.04642841468977281</v>
+        <v>0.04627761778294641</v>
       </c>
       <c r="D37" t="n">
-        <v>3760007075.434083</v>
+        <v>3747794781.725382</v>
       </c>
       <c r="E37" t="n">
-        <v>102775146.6258754</v>
+        <v>102573910.5960994</v>
       </c>
       <c r="F37" t="n">
-        <v>0.65469568</v>
+        <v>0.24786643</v>
       </c>
     </row>
     <row r="38">
@@ -1342,16 +1342,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>7.161906885477604</v>
+        <v>7.149030474303392</v>
       </c>
       <c r="D38" t="n">
-        <v>3707694191.503101</v>
+        <v>3701028118.391366</v>
       </c>
       <c r="E38" t="n">
-        <v>449384026.34232</v>
+        <v>449416600.1176429</v>
       </c>
       <c r="F38" t="n">
-        <v>0.54012228</v>
+        <v>0.4262359</v>
       </c>
     </row>
     <row r="39">
@@ -1366,16 +1366,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>192.0154633867775</v>
+        <v>191.6995528684213</v>
       </c>
       <c r="D39" t="n">
-        <v>3542060111.290632</v>
+        <v>3536232590.808321</v>
       </c>
       <c r="E39" t="n">
-        <v>77584602.34088372</v>
+        <v>77588184.84335074</v>
       </c>
       <c r="F39" t="n">
-        <v>-0.15520531</v>
+        <v>-0.31656531</v>
       </c>
     </row>
     <row r="40">
@@ -1390,16 +1390,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>460.3805311594825</v>
+        <v>459.4568611964735</v>
       </c>
       <c r="D40" t="n">
-        <v>3398039236.134146</v>
+        <v>3391221687.252054</v>
       </c>
       <c r="E40" t="n">
-        <v>211238956.3020732</v>
+        <v>211836599.103518</v>
       </c>
       <c r="F40" t="n">
-        <v>-0.43267199</v>
+        <v>-0.51182856</v>
       </c>
     </row>
     <row r="41">
@@ -1414,16 +1414,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>3.563973355837458</v>
+        <v>3.564293625131811</v>
       </c>
       <c r="D41" t="n">
-        <v>3385019945.621857</v>
+        <v>3385324133.628084</v>
       </c>
       <c r="E41" t="n">
-        <v>49512004.24273326</v>
+        <v>49614970.62176432</v>
       </c>
       <c r="F41" t="n">
-        <v>-3.20951966</v>
+        <v>-3.19365097</v>
       </c>
     </row>
     <row r="42">
@@ -1438,16 +1438,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.774734534730564</v>
+        <v>0.7733696020917132</v>
       </c>
       <c r="D42" t="n">
-        <v>3261719136.692059</v>
+        <v>3255972617.45372</v>
       </c>
       <c r="E42" t="n">
-        <v>499901985.8294385</v>
+        <v>501526645.6670145</v>
       </c>
       <c r="F42" t="n">
-        <v>2.50801386</v>
+        <v>2.40430834</v>
       </c>
     </row>
     <row r="43">
@@ -1462,64 +1462,64 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1.288994041900813</v>
+        <v>1.28553368624621</v>
       </c>
       <c r="D43" t="n">
-        <v>3145102448.647799</v>
+        <v>3136659296.322258</v>
       </c>
       <c r="E43" t="n">
-        <v>315272450.5756708</v>
+        <v>314626950.2999723</v>
       </c>
       <c r="F43" t="n">
-        <v>1.05225642</v>
+        <v>0.78394303</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Ethena</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>FIL</t>
+          <t>ENA</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>4.980843433533284</v>
+        <v>1.037312582644361</v>
       </c>
       <c r="D44" t="n">
-        <v>3056633025.492622</v>
+        <v>3047105711.517812</v>
       </c>
       <c r="E44" t="n">
-        <v>385875326.0524741</v>
+        <v>681892040.1650341</v>
       </c>
       <c r="F44" t="n">
-        <v>1.2015199</v>
+        <v>-0.61048477</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Ethena</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ENA</t>
+          <t>FIL</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1.037324456636511</v>
+        <v>4.963628554085775</v>
       </c>
       <c r="D45" t="n">
-        <v>3047140591.369751</v>
+        <v>3046068636.197654</v>
       </c>
       <c r="E45" t="n">
-        <v>680164424.7422407</v>
+        <v>386894734.0834174</v>
       </c>
       <c r="F45" t="n">
-        <v>-0.96136903</v>
+        <v>0.81052723</v>
       </c>
     </row>
     <row r="46">
@@ -1534,16 +1534,16 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.3603493302665529</v>
+        <v>0.3591466503228555</v>
       </c>
       <c r="D46" t="n">
-        <v>3003428349.542494</v>
+        <v>2993404290.289616</v>
       </c>
       <c r="E46" t="n">
-        <v>419321571.8032452</v>
+        <v>418512884.1953453</v>
       </c>
       <c r="F46" t="n">
-        <v>2.61172846</v>
+        <v>2.63779096</v>
       </c>
     </row>
     <row r="47">
@@ -1558,16 +1558,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.1179931540186514</v>
+        <v>0.117764762669642</v>
       </c>
       <c r="D47" t="n">
-        <v>2998333070.717666</v>
+        <v>2992529400.661585</v>
       </c>
       <c r="E47" t="n">
-        <v>170577982.2425398</v>
+        <v>171098889.8951296</v>
       </c>
       <c r="F47" t="n">
-        <v>-1.11496018</v>
+        <v>-1.22420974</v>
       </c>
     </row>
     <row r="48">
@@ -1582,16 +1582,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.9821736960196842</v>
+        <v>0.9788627356913631</v>
       </c>
       <c r="D48" t="n">
-        <v>2753656388.698693</v>
+        <v>2744373664.983165</v>
       </c>
       <c r="E48" t="n">
-        <v>406449367.1682094</v>
+        <v>406763196.502709</v>
       </c>
       <c r="F48" t="n">
-        <v>-1.38939815</v>
+        <v>-1.61386279</v>
       </c>
     </row>
     <row r="49">
@@ -1606,16 +1606,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>45.56693557551103</v>
+        <v>45.47082453481779</v>
       </c>
       <c r="D49" t="n">
-        <v>2734016134.530662</v>
+        <v>2728249472.089067</v>
       </c>
       <c r="E49" t="n">
-        <v>2327105.16086503</v>
+        <v>2329667.10878335</v>
       </c>
       <c r="F49" t="n">
-        <v>1.70878957</v>
+        <v>1.47674835</v>
       </c>
     </row>
     <row r="50">
@@ -1630,16 +1630,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>2.658099142545252</v>
+        <v>2.654291183886701</v>
       </c>
       <c r="D50" t="n">
-        <v>2658099142.545251</v>
+        <v>2654291183.886701</v>
       </c>
       <c r="E50" t="n">
-        <v>237713353.0731491</v>
+        <v>238087780.0917314</v>
       </c>
       <c r="F50" t="n">
-        <v>11.4205479</v>
+        <v>11.10587863</v>
       </c>
     </row>
     <row r="51">
@@ -1654,16 +1654,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>6.586070069648661</v>
+        <v>6.57679106239419</v>
       </c>
       <c r="D51" t="n">
-        <v>2574720060.166324</v>
+        <v>2571092578.851387</v>
       </c>
       <c r="E51" t="n">
-        <v>220423427.4038407</v>
+        <v>220750890.7668709</v>
       </c>
       <c r="F51" t="n">
-        <v>0.27786544</v>
+        <v>0.10150516</v>
       </c>
     </row>
   </sheetData>
@@ -1729,16 +1729,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>93868.67548097557</v>
+        <v>93593.70593424888</v>
       </c>
       <c r="D2" t="n">
-        <v>1858612352925.831</v>
+        <v>1853167919054.723</v>
       </c>
       <c r="E2" t="n">
-        <v>59599375918.81479</v>
+        <v>59748244183.16138</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.83058014</v>
+        <v>-2.16511306</v>
       </c>
     </row>
     <row r="3">
@@ -1753,16 +1753,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3374.139607770159</v>
+        <v>3352.555608610053</v>
       </c>
       <c r="D3" t="n">
-        <v>406439580895.5662</v>
+        <v>403839631695.9297</v>
       </c>
       <c r="E3" t="n">
-        <v>32434492743.43126</v>
+        <v>32513038434.96328</v>
       </c>
       <c r="F3" t="n">
-        <v>1.39229033</v>
+        <v>0.6943679699999999</v>
       </c>
     </row>
     <row r="4">
@@ -1777,16 +1777,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9986787548714428</v>
+        <v>0.9986123728111663</v>
       </c>
       <c r="D4" t="n">
-        <v>139663496085.7792</v>
+        <v>139654212669.495</v>
       </c>
       <c r="E4" t="n">
-        <v>134528538899.5783</v>
+        <v>134856672030.5432</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.05398583</v>
+        <v>-0.08507927</v>
       </c>
     </row>
     <row r="5">
@@ -1801,16 +1801,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2.195052655547284</v>
+        <v>2.190784119817687</v>
       </c>
       <c r="D5" t="n">
-        <v>125671989677.3243</v>
+        <v>125427605845.8971</v>
       </c>
       <c r="E5" t="n">
-        <v>10919366585.31427</v>
+        <v>10926323035.3287</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.94666203</v>
+        <v>-2.13208952</v>
       </c>
     </row>
     <row r="6">
@@ -1825,16 +1825,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>683.3349340120989</v>
+        <v>681.414910328032</v>
       </c>
       <c r="D6" t="n">
-        <v>98405417727.39308</v>
+        <v>98128919741.89166</v>
       </c>
       <c r="E6" t="n">
-        <v>1682453033.670772</v>
+        <v>1680950145.051784</v>
       </c>
       <c r="F6" t="n">
-        <v>3.93443311</v>
+        <v>3.53900119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>